<commit_message>
Added "requirements_progress.xlsx" to keep fixes/bugs progress up-to-date. Try/catch added to DatabaseHelper.
</commit_message>
<xml_diff>
--- a/app/src/main/assets/requirements_progress.xlsx
+++ b/app/src/main/assets/requirements_progress.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
   <si>
     <t>Req #</t>
   </si>
@@ -56,6 +56,9 @@
   </si>
   <si>
     <t>Need to replace "Attend" button with "Unattend" when the user is attending the selected event</t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
 </sst>
 </file>
@@ -450,7 +453,7 @@
   <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -546,6 +549,9 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C5" s="1"/>
+      <c r="F5" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C6" s="1"/>

</xml_diff>